<commit_message>
feature: updated the view results method and the excel sheets
</commit_message>
<xml_diff>
--- a/src/final/unblurry/unblurry_results.xlsx
+++ b/src/final/unblurry/unblurry_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="16" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="39">
   <si>
     <t>MSE</t>
   </si>
@@ -146,6 +146,9 @@
   <si>
     <t>Best</t>
   </si>
+  <si>
+    <t>Optimized</t>
+  </si>
 </sst>
 </file>
 
@@ -155,7 +158,7 @@
     <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
     <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +223,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -297,7 +308,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -342,6 +353,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="7" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -3057,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,10 +3111,10 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="29"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -3120,7 +3132,7 @@
         <f>'NN (v)'!D$8</f>
         <v>1</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="31">
         <f>'NN (v)'!G$8</f>
         <v>4.8611111111111104E-4</v>
       </c>
@@ -3165,7 +3177,7 @@
         <f>'RBF (v)'!D$8</f>
         <v>2</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="31">
         <f>'RBF (v)'!G$8</f>
         <v>2.1319444444444443E-2</v>
       </c>
@@ -3210,7 +3222,7 @@
         <f>'ESN (v)'!D$8</f>
         <v>1</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="31">
         <f>'ESN (v)'!L$8</f>
         <v>1.7824074074074076E-2</v>
       </c>
@@ -3259,7 +3271,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="32">
         <f t="shared" si="0"/>
         <v>1.7824074074074076E-2</v>
       </c>
@@ -3289,10 +3301,10 @@
       </c>
     </row>
     <row r="12" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="29"/>
+      <c r="C12" s="30"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
@@ -3310,7 +3322,7 @@
         <f>'NN (u)'!D$8</f>
         <v>1</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="31">
         <f>'NN (u)'!G$8</f>
         <v>6.134259259259259E-4</v>
       </c>
@@ -3355,7 +3367,7 @@
         <f>'RBF (u)'!D$8</f>
         <v>1</v>
       </c>
-      <c r="G14" s="30">
+      <c r="G14" s="31">
         <f>'RBF (u)'!G$8</f>
         <v>2.1296296296296299E-2</v>
       </c>
@@ -3400,33 +3412,33 @@
         <f>'ESN (u)'!D$8</f>
         <v>1</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="31">
         <f>'ESN (u)'!L$8</f>
-        <v>1.8553240740740742E-2</v>
+        <v>2.9560185185185189E-2</v>
       </c>
       <c r="H15" s="22">
         <f>'ESN (u)'!M$8</f>
-        <v>2.4383616789405101E-2</v>
+        <v>2.3468715974459702E-2</v>
       </c>
       <c r="I15" s="22">
         <f>'ESN (u)'!N$8</f>
-        <v>2.3277842710800099E-2</v>
+        <v>2.2691396564518199E-2</v>
       </c>
       <c r="J15" s="10">
         <f>'ESN (u)'!O$8</f>
-        <v>0.16359244531214631</v>
+        <v>0.15745427217615662</v>
       </c>
       <c r="K15" s="10">
         <f>'ESN (u)'!P$8</f>
-        <v>0.40446562933350261</v>
+        <v>0.39680508083460403</v>
       </c>
       <c r="L15" s="10">
         <f>'ESN (u)'!Q$8</f>
-        <v>0.30843764873477414</v>
+        <v>0.15745427217615662</v>
       </c>
       <c r="M15" s="10">
         <f>'ESN (u)'!R$8</f>
-        <v>0.55537163119372068</v>
+        <v>0.39680508083460403</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
@@ -3449,33 +3461,33 @@
         <f t="shared" ref="F16" si="3">INDEX(F13:F15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
         <v>1</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="32">
         <f t="shared" ref="G16" si="4">INDEX(G13:G15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
-        <v>1.8553240740740742E-2</v>
+        <v>2.9560185185185189E-2</v>
       </c>
       <c r="H16" s="7">
         <f t="shared" ref="H16" si="5">INDEX(H13:H15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
-        <v>2.4383616789405101E-2</v>
+        <v>2.3468715974459702E-2</v>
       </c>
       <c r="I16" s="7">
         <f t="shared" ref="I16" si="6">INDEX(I13:I15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
-        <v>2.3277842710800099E-2</v>
+        <v>2.2691396564518199E-2</v>
       </c>
       <c r="J16" s="8">
         <f t="shared" ref="J16" si="7">INDEX(J13:J15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
-        <v>0.16359244531214631</v>
+        <v>0.15745427217615662</v>
       </c>
       <c r="K16" s="8">
         <f t="shared" ref="K16" si="8">INDEX(K13:K15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
-        <v>0.40446562933350261</v>
+        <v>0.39680508083460403</v>
       </c>
       <c r="L16" s="8">
         <f t="shared" ref="L16" si="9">INDEX(L13:L15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
-        <v>0.30843764873477414</v>
+        <v>0.15745427217615662</v>
       </c>
       <c r="M16" s="8">
         <f t="shared" ref="M16" si="10">INDEX(M13:M15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
-        <v>0.55537163119372068</v>
+        <v>0.39680508083460403</v>
       </c>
     </row>
   </sheetData>
@@ -25031,8 +25043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25106,59 +25118,59 @@
       </c>
       <c r="E8" s="7">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H8" s="7">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="0"/>
-        <v>5.0000000000000004E-6</v>
+        <v>5.0000000000000003E-10</v>
       </c>
       <c r="L8" s="15">
         <f t="shared" si="0"/>
-        <v>1.8553240740740742E-2</v>
+        <v>2.9560185185185189E-2</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" si="0"/>
-        <v>2.4383616789405101E-2</v>
+        <v>2.3468715974459702E-2</v>
       </c>
       <c r="N8" s="7">
         <f t="shared" si="0"/>
-        <v>2.3277842710800099E-2</v>
+        <v>2.2691396564518199E-2</v>
       </c>
       <c r="O8" s="8">
         <f t="shared" si="0"/>
-        <v>0.16359244531214631</v>
+        <v>0.15745427217615662</v>
       </c>
       <c r="P8" s="8">
         <f t="shared" si="0"/>
-        <v>0.40446562933350261</v>
+        <v>0.39680508083460403</v>
       </c>
       <c r="Q8" s="8">
         <f t="shared" si="0"/>
-        <v>0.30843764873477414</v>
+        <v>0.15745427217615662</v>
       </c>
       <c r="R8" s="8">
         <f t="shared" si="0"/>
-        <v>0.55537163119372068</v>
+        <v>0.39680508083460403</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -25647,13 +25659,13 @@
       </c>
       <c r="T16" s="20"/>
     </row>
-    <row r="17" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T17" s="20"/>
     </row>
-    <row r="18" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T18" s="20"/>
     </row>
-    <row r="19" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>33</v>
       </c>
@@ -25665,40 +25677,89 @@
       </c>
       <c r="T19" s="20"/>
     </row>
-    <row r="20" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20" s="20"/>
       <c r="T20" s="20"/>
     </row>
-    <row r="21" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C21" s="1">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>200</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24">
+        <v>5.0000000000000003E-10</v>
+      </c>
+      <c r="L21" s="19">
+        <v>2.9560185185185189E-2</v>
+      </c>
+      <c r="M21" s="9">
+        <v>2.3468715974459702E-2</v>
+      </c>
+      <c r="N21" s="9">
+        <v>2.2691396564518199E-2</v>
+      </c>
+      <c r="O21" s="10">
+        <f>M21/$C$2</f>
+        <v>0.15745427217615662</v>
+      </c>
+      <c r="P21" s="10">
+        <f>SQRT(O21)</f>
+        <v>0.39680508083460403</v>
+      </c>
+      <c r="Q21" s="10">
+        <f>M21/$C$2</f>
+        <v>0.15745427217615662</v>
+      </c>
+      <c r="R21" s="10">
+        <f>SQRT(Q21)</f>
+        <v>0.39680508083460403</v>
+      </c>
       <c r="T21" s="20"/>
     </row>
-    <row r="22" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T22" s="20"/>
     </row>
-    <row r="23" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T23" s="20"/>
     </row>
-    <row r="24" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T24" s="20"/>
     </row>
-    <row r="25" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T25" s="20"/>
     </row>
-    <row r="26" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T26" s="20"/>
     </row>
-    <row r="27" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T27" s="20"/>
     </row>
-    <row r="29" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T29" s="14"/>
     </row>
-    <row r="30" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T30" s="14"/>
     </row>
-    <row r="31" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T31" s="14"/>
     </row>
-    <row r="32" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T32" s="14"/>
     </row>
     <row r="33" spans="20:20" x14ac:dyDescent="0.25">

</xml_diff>